<commit_message>
Update reference to tutorial
</commit_message>
<xml_diff>
--- a/Einsatzsuche.xlsx
+++ b/Einsatzsuche.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Structured" sheetId="1" state="visible" r:id="rId1"/>
@@ -873,13 +873,13 @@
       </c>
       <c r="R1" s="9"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="129" customHeight="1">
+    <row r="2" s="1" customFormat="1" ht="181.5" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="11" t="str">
         <f>"-"&amp;_xlfn.TEXTJOIN("
--",TRUE,Tutorial!A1:A9)</f>
+-",TRUE,Tutorial!A1:A20)</f>
         <v xml:space="preserve">-Einsatzsuche von ZiviConnect öffnen
 -Beliebige Filter einstellen
 -Die f12 taste oder ctrl+shift+i drücken
@@ -888,7 +888,10 @@
 -In den Developer Tools den neuen Eintrag "search" in der Tabelle rechts klicken
 -Die Antwort Speichern
 -Die Datei zu CSV Konvertieren
--Das Resultat im "Suchresultate" Arbeitsblatt einfügen</v>
+-Das Resultat im "Suchresultate" Arbeitsblatt einfügen
+-Einzelne Pflichtenhefter gleichermassen herunterladen
+-Diese mit dem Python Script einlesen
+-Resultat im "Pflichtenhefte" Arbeitsblatt einfügen</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -38574,8 +38577,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="26" width="9.140625"/>
-    <col min="2" max="16384" style="26" width="9.140625"/>
+    <col min="1" max="16384" style="26" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">

</xml_diff>